<commit_message>
cascadeGrouping working (missing documentation)
</commit_message>
<xml_diff>
--- a/overviewFile.xlsx
+++ b/overviewFile.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,6 +470,55 @@
       </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>event 2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>event 3</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>event 4</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>event 5</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>event 6</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>event 7</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="n"/>
+      <c r="V1" s="1" t="n"/>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>event 8</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="n"/>
+      <c r="Y1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr"/>
@@ -488,6 +537,111 @@
           <t>Host</t>
         </is>
       </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="F2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="G2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="T2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="U2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="V2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
+      <c r="W2" s="1" t="inlineStr">
+        <is>
+          <t>boy members</t>
+        </is>
+      </c>
+      <c r="X2" s="1" t="inlineStr">
+        <is>
+          <t>girl members</t>
+        </is>
+      </c>
+      <c r="Y2" s="1" t="inlineStr">
+        <is>
+          <t>Host</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -497,16 +651,107 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[9, 14]</t>
+          <t>[33, 46, 62]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[0, 4, 8]</t>
+          <t>[0, 13]</t>
         </is>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>[44, 58, 62]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>[9, 23]</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>23</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>[33, 46, 62]</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>[0, 13]</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>[44, 58, 62]</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>[9, 23]</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
         <v>9</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>[33, 46, 62]</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>[0, 13]</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>[44, 58, 62]</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>[9, 23]</t>
+        </is>
+      </c>
+      <c r="S4" t="n">
+        <v>44</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>[33, 46, 62]</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>[0, 13]</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v>46</v>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>[57, 45, 33]</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>[27, 23]</t>
+        </is>
+      </c>
+      <c r="Y4" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -517,16 +762,107 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[10, 15, 19]</t>
+          <t>[34, 47, 61]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[1, 5]</t>
+          <t>[1, 14]</t>
         </is>
       </c>
       <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>[45, 46, 61]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>[10, 24]</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[34, 47, 61]</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>[1, 14]</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>[45, 46, 61]</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>[10, 24]</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
         <v>10</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>[34, 47, 61]</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>[1, 14]</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>[45, 46, 61]</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>[10, 24]</t>
+        </is>
+      </c>
+      <c r="S5" t="n">
+        <v>45</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>[34, 47, 61]</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>[1, 14]</t>
+        </is>
+      </c>
+      <c r="V5" t="n">
+        <v>47</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>[58, 46, 34]</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>[26, 11]</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -537,16 +873,107 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[11, 16]</t>
+          <t>[35, 48, 60]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[2, 6]</t>
+          <t>[2, 15]</t>
         </is>
       </c>
       <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>[33, 47, 60]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>[11, 25]</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>25</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>[35, 48, 60]</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>[2, 15]</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>35</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>[33, 47, 60]</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>[11, 25]</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
         <v>11</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>[35, 48, 60]</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>[2, 15]</t>
+        </is>
+      </c>
+      <c r="P6" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>[33, 47, 60]</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>[11, 25]</t>
+        </is>
+      </c>
+      <c r="S6" t="n">
+        <v>33</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>[35, 48, 60]</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>[2, 15]</t>
+        </is>
+      </c>
+      <c r="V6" t="n">
+        <v>48</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>[62, 47, 35]</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>[24, 12]</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="7">
@@ -557,16 +984,107 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[12, 17]</t>
+          <t>[36, 49, 59]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>[3, 7]</t>
+          <t>[3, 16]</t>
         </is>
       </c>
       <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>[34, 48, 59]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>[12, 13]</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>13</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>[36, 49, 59]</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>[3, 16]</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>36</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>[34, 48, 59]</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>[12, 13]</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
         <v>12</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>[36, 49, 59]</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>[3, 16]</t>
+        </is>
+      </c>
+      <c r="P7" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>[34, 48, 59]</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>[12, 13]</t>
+        </is>
+      </c>
+      <c r="S7" t="n">
+        <v>34</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>[36, 49, 59]</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>[3, 16]</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>49</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>[61, 48, 36]</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>[25, 0]</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -577,21 +1095,1007 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[13, 18, 21, 20]</t>
+          <t>[37, 50]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[4, 17, 32]</t>
         </is>
       </c>
       <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>[35, 49]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>[0, 14, 32]</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>14</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>[37, 50]</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>[4, 17, 32]</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>37</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>[35, 49]</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>[0, 14, 32]</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>[37, 50]</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>[4, 17, 32]</t>
+        </is>
+      </c>
+      <c r="P8" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>[35, 49]</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>[0, 14, 32]</t>
+        </is>
+      </c>
+      <c r="S8" t="n">
+        <v>35</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>[37, 50]</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>[4, 17, 32]</t>
+        </is>
+      </c>
+      <c r="V8" t="n">
+        <v>50</v>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>[60, 49]</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>[13, 1, 4]</t>
+        </is>
+      </c>
+      <c r="Y8" t="n">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Group_5</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[38, 51]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[5, 18, 31]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>[36, 50]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>[1, 15, 31]</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>15</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[38, 51]</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>[5, 18, 31]</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>38</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>[36, 50]</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>[1, 15, 31]</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>1</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>[38, 51]</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>[5, 18, 31]</t>
+        </is>
+      </c>
+      <c r="P9" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>[36, 50]</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>[1, 15, 31]</t>
+        </is>
+      </c>
+      <c r="S9" t="n">
+        <v>36</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>[38, 51]</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>[5, 18, 31]</t>
+        </is>
+      </c>
+      <c r="V9" t="n">
+        <v>51</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>[59, 37]</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>[14, 2, 5]</t>
+        </is>
+      </c>
+      <c r="Y9" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Group_6</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>[39, 52]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>[6, 19, 30]</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>[37, 51]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>[2, 16, 30]</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>16</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>[39, 52]</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>[6, 19, 30]</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>39</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>[37, 51]</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>[2, 16, 30]</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>[39, 52]</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>[6, 19, 30]</t>
+        </is>
+      </c>
+      <c r="P10" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>[37, 51]</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>[2, 16, 30]</t>
+        </is>
+      </c>
+      <c r="S10" t="n">
+        <v>37</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>[39, 52]</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>[6, 19, 30]</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v>52</v>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>[50, 38]</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>[15, 3, 6]</t>
+        </is>
+      </c>
+      <c r="Y10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Group_7</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[40, 53]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>[7, 20, 29]</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>[38, 52]</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>[3, 17, 29]</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>17</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>[40, 53]</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>[7, 20, 29]</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>40</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>[38, 52]</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>[3, 17, 29]</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>[40, 53]</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>[7, 20, 29]</t>
+        </is>
+      </c>
+      <c r="P11" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>[38, 52]</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>[3, 17, 29]</t>
+        </is>
+      </c>
+      <c r="S11" t="n">
+        <v>38</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>[40, 53]</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>[7, 20, 29]</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>53</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>[51, 39]</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>[16, 17, 7]</t>
+        </is>
+      </c>
+      <c r="Y11" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Group_8</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[41, 54]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>[8, 21, 28]</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>8</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>[39, 53]</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>[4, 18, 28]</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>18</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>[41, 54]</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>[8, 21, 28]</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>41</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>[39, 53]</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>[4, 18, 28]</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>4</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>[41, 54]</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>[8, 21, 28]</t>
+        </is>
+      </c>
+      <c r="P12" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>[39, 53]</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>[4, 18, 28]</t>
+        </is>
+      </c>
+      <c r="S12" t="n">
+        <v>39</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>[41, 54]</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>[8, 21, 28]</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>54</v>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>[52, 40]</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>[32, 18, 8]</t>
+        </is>
+      </c>
+      <c r="Y12" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Group_9</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>[42, 55]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>[9, 22, 27]</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[40, 54]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[5, 19, 27]</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>19</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>[42, 55]</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>[9, 22, 27]</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>42</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>[40, 54]</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>[5, 19, 27]</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>[42, 55]</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>[9, 22, 27]</t>
+        </is>
+      </c>
+      <c r="P13" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>[40, 54]</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>[5, 19, 27]</t>
+        </is>
+      </c>
+      <c r="S13" t="n">
+        <v>40</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>[42, 55]</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>[9, 22, 27]</t>
+        </is>
+      </c>
+      <c r="V13" t="n">
+        <v>55</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>[53, 41]</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>[31, 19, 9]</t>
+        </is>
+      </c>
+      <c r="Y13" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Group_10</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>[43, 56]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>[10, 23, 26]</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>10</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[41, 55]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>[6, 20, 26]</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>[43, 56]</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>[10, 23, 26]</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>43</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>[41, 55]</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>[6, 20, 26]</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>6</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>[43, 56]</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>[10, 23, 26]</t>
+        </is>
+      </c>
+      <c r="P14" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>[41, 55]</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>[6, 20, 26]</t>
+        </is>
+      </c>
+      <c r="S14" t="n">
+        <v>41</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>[43, 56]</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>[10, 23, 26]</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>56</v>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>[54, 42]</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>[30, 20, 10]</t>
+        </is>
+      </c>
+      <c r="Y14" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Group_11</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[44, 57]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[11, 24]</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>11</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[42, 56]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[7, 21]</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>21</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>[44, 57]</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>[11, 24]</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>44</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>[42, 56]</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>[7, 21]</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>7</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>[44, 57]</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>[11, 24]</t>
+        </is>
+      </c>
+      <c r="P15" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>[42, 56]</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>[7, 21]</t>
+        </is>
+      </c>
+      <c r="S15" t="n">
+        <v>42</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>[44, 57]</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>[11, 24]</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>57</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>[55, 43]</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
+        <is>
+          <t>[29, 21]</t>
+        </is>
+      </c>
+      <c r="Y15" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Group_12</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>[45, 58]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>[12, 25]</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>12</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[43, 57]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[8, 22]</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>22</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>[45, 58]</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>[12, 25]</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>45</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>[43, 57]</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>[8, 22]</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>8</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>[45, 58]</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>[12, 25]</t>
+        </is>
+      </c>
+      <c r="P16" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>[43, 57]</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>[8, 22]</t>
+        </is>
+      </c>
+      <c r="S16" t="n">
+        <v>43</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>[45, 58]</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>[12, 25]</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>58</v>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>[56, 44]</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>[28, 22]</t>
+        </is>
+      </c>
+      <c r="Y16" t="n">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>